<commit_message>
Temporary commit of changes in the code
</commit_message>
<xml_diff>
--- a/General/Fuel_rack_analysis.xlsx
+++ b/General/Fuel_rack_analysis.xlsx
@@ -140,13 +140,13 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2586,7 +2586,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2607,6 +2607,10 @@
         <f>INDEX(LINEST($M$9:$M$23,$C$9:$C$23),1)</f>
         <v>28.278799590715863</v>
       </c>
+      <c r="H1">
+        <f>INDEX(LINEST($M$4:$M$8,$C$4:$C$8),1)</f>
+        <v>24.232538802060759</v>
+      </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -2623,6 +2627,10 @@
         <v>1154.675</v>
       </c>
       <c r="G2">
+        <f>INDEX(LINEST($M$9:$M$23,$C$9:$C$23),2)</f>
+        <v>-159.61163790710066</v>
+      </c>
+      <c r="H2">
         <f>INDEX(LINEST($M$9:$M$23,$C$9:$C$23),2)</f>
         <v>-159.61163790710066</v>
       </c>
@@ -2680,7 +2688,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
@@ -2721,7 +2729,7 @@
         <f>I4*$E$2</f>
         <v>638.75638297872342</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="2">
         <f>ABS((O4-E4)/E4)</f>
         <v>0.89936480219662029</v>
       </c>
@@ -2729,13 +2737,13 @@
         <f>$E$2*($G$2+$G$1*C4)/($G$2+$G$1*$C$2)*J4</f>
         <v>358.05677337470797</v>
       </c>
-      <c r="R4" s="4">
+      <c r="R4" s="2">
         <f>ABS((Q4-E4)/E4)</f>
         <v>6.4694538729431941E-2</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="4"/>
       <c r="B5">
         <v>0.5</v>
       </c>
@@ -2774,7 +2782,7 @@
         <f t="shared" ref="O5:O8" si="4">I5*$E$2</f>
         <v>859.86436170212755</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="2">
         <f t="shared" ref="P5:P8" si="5">ABS((O5-E5)/E5)</f>
         <v>0.46334983271294677</v>
       </c>
@@ -2782,13 +2790,13 @@
         <f t="shared" ref="Q5:Q23" si="6">$E$2*($G$2+$G$1*C5)/($G$2+$G$1*$C$2)*J5</f>
         <v>650.78523758232939</v>
       </c>
-      <c r="R5" s="4">
+      <c r="R5" s="2">
         <f t="shared" ref="R5:R23" si="7">ABS((Q5-E5)/E5)</f>
         <v>0.1075310374103631</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="4"/>
       <c r="B6">
         <v>0.75</v>
       </c>
@@ -2827,7 +2835,7 @@
         <f t="shared" si="4"/>
         <v>1031.8372340425531</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="2">
         <f t="shared" si="5"/>
         <v>0.23042837353035181</v>
       </c>
@@ -2835,13 +2843,13 @@
         <f t="shared" si="6"/>
         <v>921.68574022079918</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6" s="2">
         <f t="shared" si="7"/>
         <v>9.9076723373240097E-2</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="4"/>
       <c r="B7">
         <v>0.85</v>
       </c>
@@ -2880,7 +2888,7 @@
         <f t="shared" si="4"/>
         <v>1130.1074468085105</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="2">
         <f t="shared" si="5"/>
         <v>0.18571760235915485</v>
       </c>
@@ -2888,13 +2896,13 @@
         <f t="shared" si="6"/>
         <v>1068.1632472531537</v>
       </c>
-      <c r="R7" s="4">
+      <c r="R7" s="2">
         <f t="shared" si="7"/>
         <v>0.12072526204296893</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="4"/>
       <c r="B8">
         <v>1</v>
       </c>
@@ -2933,7 +2941,7 @@
         <f t="shared" si="4"/>
         <v>1252.9452127659572</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P8" s="2">
         <f t="shared" si="5"/>
         <v>9.811149234527361E-2</v>
       </c>
@@ -2941,13 +2949,13 @@
         <f t="shared" si="6"/>
         <v>1266.3570791006173</v>
       </c>
-      <c r="R8" s="4">
+      <c r="R8" s="2">
         <f t="shared" si="7"/>
         <v>0.10986597642473031</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B9">
@@ -2988,7 +2996,7 @@
         <f>I9*$E$2</f>
         <v>589.62127659574458</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="2">
         <f>ABS((O9-E9)/E9)</f>
         <v>0.84776332370963503</v>
       </c>
@@ -2996,13 +3004,13 @@
         <f t="shared" si="6"/>
         <v>322.87691845801351</v>
       </c>
-      <c r="R9" s="4">
+      <c r="R9" s="2">
         <f t="shared" si="7"/>
         <v>1.1836159379547111E-2</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="4"/>
       <c r="B10">
         <v>0.5</v>
       </c>
@@ -3041,7 +3049,7 @@
         <f t="shared" ref="O10:O13" si="12">I10*$E$2</f>
         <v>786.16170212765951</v>
       </c>
-      <c r="P10" s="4">
+      <c r="P10" s="2">
         <f t="shared" ref="P10:P13" si="13">ABS((O10-E10)/E10)</f>
         <v>0.33883123659342551</v>
       </c>
@@ -3049,13 +3057,13 @@
         <f t="shared" si="6"/>
         <v>584.2785594779117</v>
       </c>
-      <c r="R10" s="4">
+      <c r="R10" s="2">
         <f t="shared" si="7"/>
         <v>4.9752052487880552E-3</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="4"/>
       <c r="B11">
         <v>0.75</v>
       </c>
@@ -3094,7 +3102,7 @@
         <f t="shared" si="12"/>
         <v>933.5670212765956</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P11" s="2">
         <f t="shared" si="13"/>
         <v>0.11590607372292083</v>
       </c>
@@ -3102,13 +3110,13 @@
         <f t="shared" si="6"/>
         <v>820.27841239743861</v>
       </c>
-      <c r="R11" s="4">
+      <c r="R11" s="2">
         <f t="shared" si="7"/>
         <v>1.9509428164668191E-2</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="4"/>
       <c r="B12">
         <v>0.85</v>
       </c>
@@ -3147,7 +3155,7 @@
         <f t="shared" si="12"/>
         <v>1007.2696808510639</v>
       </c>
-      <c r="P12" s="4">
+      <c r="P12" s="2">
         <f t="shared" si="13"/>
         <v>5.0990902390509067E-2</v>
       </c>
@@ -3155,13 +3163,13 @@
         <f t="shared" si="6"/>
         <v>935.81998351892207</v>
       </c>
-      <c r="R12" s="4">
+      <c r="R12" s="2">
         <f t="shared" si="7"/>
         <v>2.3560117363395142E-2</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="4"/>
       <c r="B13">
         <v>1</v>
       </c>
@@ -3200,7 +3208,7 @@
         <f t="shared" si="12"/>
         <v>1154.675</v>
       </c>
-      <c r="P13" s="4">
+      <c r="P13" s="2">
         <f t="shared" si="13"/>
         <v>8.9477298086000825E-3</v>
       </c>
@@ -3208,13 +3216,13 @@
         <f t="shared" si="6"/>
         <v>1154.675</v>
       </c>
-      <c r="R13" s="4">
+      <c r="R13" s="2">
         <f t="shared" si="7"/>
         <v>8.9477298086000825E-3</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B14">
@@ -3255,7 +3263,7 @@
         <f>I14*$E$2</f>
         <v>614.188829787234</v>
       </c>
-      <c r="P14" s="4">
+      <c r="P14" s="2">
         <f>ABS((O14-E14)/E14)</f>
         <v>0.75232191094788592</v>
       </c>
@@ -3263,13 +3271,13 @@
         <f t="shared" si="6"/>
         <v>340.46684591636074</v>
       </c>
-      <c r="R14" s="4">
+      <c r="R14" s="2">
         <f t="shared" si="7"/>
         <v>2.8625261294263224E-2</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="4"/>
       <c r="B15">
         <v>0.5</v>
       </c>
@@ -3308,7 +3316,7 @@
         <f t="shared" ref="O15:O18" si="18">I15*$E$2</f>
         <v>786.16170212765951</v>
       </c>
-      <c r="P15" s="4">
+      <c r="P15" s="2">
         <f t="shared" ref="P15:P18" si="19">ABS((O15-E15)/E15)</f>
         <v>0.33951559401543624</v>
       </c>
@@ -3316,13 +3324,13 @@
         <f t="shared" si="6"/>
         <v>584.2785594779117</v>
       </c>
-      <c r="R15" s="4">
+      <c r="R15" s="2">
         <f t="shared" si="7"/>
         <v>4.466588042406335E-3</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="4"/>
       <c r="B16">
         <v>0.75</v>
       </c>
@@ -3361,7 +3369,7 @@
         <f t="shared" si="18"/>
         <v>958.13457446808502</v>
       </c>
-      <c r="P16" s="4">
+      <c r="P16" s="2">
         <f t="shared" si="19"/>
         <v>0.13428977680606721</v>
       </c>
@@ -3369,13 +3377,13 @@
         <f t="shared" si="6"/>
         <v>845.63024435327895</v>
       </c>
-      <c r="R16" s="4">
+      <c r="R16" s="2">
         <f t="shared" si="7"/>
         <v>1.1012718755521586E-3</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="4"/>
       <c r="B17">
         <v>0.85</v>
       </c>
@@ -3414,7 +3422,7 @@
         <f t="shared" si="18"/>
         <v>1031.8372340425531</v>
       </c>
-      <c r="P17" s="4">
+      <c r="P17" s="2">
         <f t="shared" si="19"/>
         <v>5.7752162011843224E-2</v>
       </c>
@@ -3422,13 +3430,13 @@
         <f t="shared" si="6"/>
         <v>962.28863626576822</v>
       </c>
-      <c r="R17" s="4">
+      <c r="R17" s="2">
         <f t="shared" si="7"/>
         <v>1.3543171434373943E-2</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
+      <c r="A18" s="4"/>
       <c r="B18">
         <v>1</v>
       </c>
@@ -3467,7 +3475,7 @@
         <f t="shared" si="18"/>
         <v>1154.675</v>
       </c>
-      <c r="P18" s="4">
+      <c r="P18" s="2">
         <f t="shared" si="19"/>
         <v>2.3220486111110716E-3</v>
       </c>
@@ -3475,13 +3483,13 @@
         <f t="shared" si="6"/>
         <v>1154.675</v>
       </c>
-      <c r="R18" s="4">
+      <c r="R18" s="2">
         <f t="shared" si="7"/>
         <v>2.3220486111110716E-3</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B19">
@@ -3522,7 +3530,7 @@
         <f>I19*$E$2</f>
         <v>589.62127659574458</v>
       </c>
-      <c r="P19" s="4">
+      <c r="P19" s="2">
         <f>ABS((O19-E19)/E19)</f>
         <v>0.80754529918989759</v>
       </c>
@@ -3530,13 +3538,13 @@
         <f t="shared" si="6"/>
         <v>322.87691845801351</v>
       </c>
-      <c r="R19" s="4">
+      <c r="R19" s="2">
         <f t="shared" si="7"/>
         <v>1.0187251814796084E-2</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="4"/>
       <c r="B20">
         <v>0.5</v>
       </c>
@@ -3575,7 +3583,7 @@
         <f t="shared" ref="O20:O23" si="24">I20*$E$2</f>
         <v>761.59414893617009</v>
       </c>
-      <c r="P20" s="4">
+      <c r="P20" s="2">
         <f t="shared" ref="P20:P23" si="25">ABS((O20-E20)/E20)</f>
         <v>0.31286700385480098</v>
       </c>
@@ -3583,13 +3591,13 @@
         <f t="shared" si="6"/>
         <v>562.10966677643921</v>
       </c>
-      <c r="R20" s="4">
+      <c r="R20" s="2">
         <f t="shared" si="7"/>
         <v>3.1012468925290138E-2</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="4"/>
       <c r="B21">
         <v>0.75</v>
       </c>
@@ -3628,7 +3636,7 @@
         <f t="shared" si="24"/>
         <v>933.5670212765956</v>
       </c>
-      <c r="P21" s="4">
+      <c r="P21" s="2">
         <f t="shared" si="25"/>
         <v>0.11244878607792605</v>
       </c>
@@ -3636,13 +3644,13 @@
         <f t="shared" si="6"/>
         <v>820.27841239743861</v>
       </c>
-      <c r="R21" s="4">
+      <c r="R21" s="2">
         <f t="shared" si="7"/>
         <v>2.2547173024977871E-2</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+      <c r="A22" s="4"/>
       <c r="B22">
         <v>0.85</v>
       </c>
@@ -3681,7 +3689,7 @@
         <f t="shared" si="24"/>
         <v>1031.8372340425531</v>
       </c>
-      <c r="P22" s="4">
+      <c r="P22" s="2">
         <f t="shared" si="25"/>
         <v>6.8043923033384787E-2</v>
       </c>
@@ -3689,13 +3697,13 @@
         <f t="shared" si="6"/>
         <v>962.28863626576822</v>
       </c>
-      <c r="R22" s="4">
+      <c r="R22" s="2">
         <f t="shared" si="7"/>
         <v>3.9451027163148788E-3</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="4"/>
       <c r="B23">
         <v>1</v>
       </c>
@@ -3734,7 +3742,7 @@
         <f t="shared" si="24"/>
         <v>1130.1074468085105</v>
       </c>
-      <c r="P23" s="4">
+      <c r="P23" s="2">
         <f t="shared" si="25"/>
         <v>2.6273094254255884E-2</v>
       </c>
@@ -3742,7 +3750,7 @@
         <f t="shared" si="6"/>
         <v>1126.7544802248458</v>
       </c>
-      <c r="R23" s="4">
+      <c r="R23" s="2">
         <f t="shared" si="7"/>
         <v>2.9162088381142617E-2</v>
       </c>

</xml_diff>